<commit_message>
added code to generate map with circles
</commit_message>
<xml_diff>
--- a/Data/Examples.xlsx
+++ b/Data/Examples.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Lat</t>
   </si>
@@ -26,6 +26,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Occupied</t>
+  </si>
+  <si>
     <t>62°50'22.66"N</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
     <t>Helags</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>63°49'50.28"N</t>
   </si>
   <si>
@@ -51,6 +57,9 @@
   </si>
   <si>
     <t>Borgafjäll</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
   <si>
     <t>65°49'19.57"N</t>
@@ -270,10 +279,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C16" activeCellId="0" pane="topLeft" sqref="C16"/>
+      <selection activeCell="H12" activeCellId="0" pane="topLeft" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -282,7 +291,7 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -292,93 +301,120 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>